<commit_message>
AVALIAÇÃO AULA 3 E TESTES AULA 2
</commit_message>
<xml_diff>
--- a/ESTATÍSTICA PARA CIÊNCIA DE DADOS/AULA 2/TESTE - PROB XÍCARA.xlsx
+++ b/ESTATÍSTICA PARA CIÊNCIA DE DADOS/AULA 2/TESTE - PROB XÍCARA.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilo\OneDrive\MBA - USP\ESTATÍSTICA PARA CIÊNCIA DE DADOS\AULA 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40C10CBC-B9EB-4304-AC5A-1CEEFCD5CFA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A81DAB-622B-4CCE-8A8C-75290E6BA5CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{31AC6215-A394-4A58-8C34-5CC7834DE709}"/>
+    <workbookView xWindow="5460" yWindow="1275" windowWidth="15375" windowHeight="7995" activeTab="1" xr2:uid="{31AC6215-A394-4A58-8C34-5CC7834DE709}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -435,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F864A550-6EB3-48B0-A6FA-521B6582B1AB}">
-  <dimension ref="B1:J7"/>
+  <dimension ref="B1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,57 +465,21 @@
       </c>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
         <v>0.5</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <f>4*(0.5^3)*0.5</f>
-        <v>0.25</v>
-      </c>
-      <c r="H2" t="str">
-        <f>RIGHT(F2,1)</f>
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <f>H2*G2</f>
-        <v>0.75</v>
-      </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
         <v>0.5</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <f>(0.5^4)</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H6" si="0">RIGHT(F3,1)</f>
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I6" si="1">H3*G3</f>
-        <v>0.25</v>
       </c>
       <c r="J3" s="2"/>
     </row>
@@ -526,15 +491,15 @@
         <v>2</v>
       </c>
       <c r="G4">
-        <f>(1-0.5)^4</f>
+        <f>((1-0.5)^4)*(0.5^0)</f>
         <v>6.25E-2</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H3:H6" si="0">RIGHT(F4,1)</f>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I3:I6" si="1">H4*G4</f>
         <v>0</v>
       </c>
       <c r="J4" s="2"/>
@@ -581,13 +546,95 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H7" t="s">
+    <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>4*(0.5^3)*(1- 0.5)^1</f>
+        <v>0.25</v>
+      </c>
+      <c r="H7" t="str">
+        <f>RIGHT(F7,1)</f>
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <f>H7*G7</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f>(0.5^4)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H8" t="str">
+        <f>RIGHT(F8,1)</f>
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <f>H8*G8</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
         <v>13</v>
       </c>
-      <c r="I7">
-        <f>SUM(I2:I6)</f>
+      <c r="I9">
+        <f>SUM(I4:I8)</f>
         <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28504EA-374C-4FAE-8AAF-C4123A2C9CBD}">
+  <dimension ref="B2:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <f>B4^B2</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <f>(1-B4)^(B3-B2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <f>D3*D2</f>
+        <v>6.25E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testes adicionais de probabilidade
</commit_message>
<xml_diff>
--- a/ESTATÍSTICA PARA CIÊNCIA DE DADOS/AULA 2/TESTE - PROB XÍCARA.xlsx
+++ b/ESTATÍSTICA PARA CIÊNCIA DE DADOS/AULA 2/TESTE - PROB XÍCARA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilo\OneDrive\MBA - USP\ESTATÍSTICA PARA CIÊNCIA DE DADOS\AULA 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A81DAB-622B-4CCE-8A8C-75290E6BA5CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46DB537-B1A4-4EEB-A198-6936E1B7407B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="1275" windowWidth="15375" windowHeight="7995" activeTab="1" xr2:uid="{31AC6215-A394-4A58-8C34-5CC7834DE709}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{31AC6215-A394-4A58-8C34-5CC7834DE709}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -436,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F864A550-6EB3-48B0-A6FA-521B6582B1AB}">
-  <dimension ref="B1:J9"/>
+  <dimension ref="B1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +502,10 @@
         <f t="shared" ref="I3:I6" si="1">H4*G4</f>
         <v>0</v>
       </c>
-      <c r="J4" s="2"/>
+      <c r="J4" s="2">
+        <f>H4^2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="E5" s="2" t="s">
@@ -523,7 +526,10 @@
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="J5" s="2"/>
+      <c r="J5" s="2">
+        <f t="shared" ref="J5:J8" si="2">H5^2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
@@ -544,7 +550,10 @@
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
@@ -565,6 +574,10 @@
         <f>H7*G7</f>
         <v>0.75</v>
       </c>
+      <c r="J7" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="E8" s="2" t="s">
@@ -585,6 +598,10 @@
         <f>H8*G8</f>
         <v>0.25</v>
       </c>
+      <c r="J8" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
@@ -593,6 +610,16 @@
       <c r="I9">
         <f>SUM(I4:I8)</f>
         <v>2</v>
+      </c>
+      <c r="J9" s="2">
+        <f>AVERAGE(J4:J8)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="2">
+        <f>_xlfn.VAR.P(J4:J8)</f>
+        <v>34.799999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -604,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28504EA-374C-4FAE-8AAF-C4123A2C9CBD}">
   <dimension ref="B2:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>